<commit_message>
Auto update: 2025-11-29 02:59:41
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>날짜</t>
   </si>
@@ -34,61 +34,82 @@
     <t>5일수익률</t>
   </si>
   <si>
-    <t>점수</t>
-  </si>
-  <si>
-    <t>3일확률</t>
-  </si>
-  <si>
-    <t>5일확률</t>
-  </si>
-  <si>
-    <t>10일확률</t>
+    <t>점수(룰)</t>
+  </si>
+  <si>
+    <t>3일상승확률(%)</t>
+  </si>
+  <si>
+    <t>5일상승확률(%)</t>
+  </si>
+  <si>
+    <t>10일상승확률(%)</t>
+  </si>
+  <si>
+    <t>최종점수</t>
+  </si>
+  <si>
+    <t>예측방식</t>
   </si>
   <si>
     <t>판단</t>
   </si>
   <si>
-    <t>2025-11-28</t>
+    <t>MACRO_SCORE</t>
+  </si>
+  <si>
+    <t>MACRO_SIGNAL</t>
+  </si>
+  <si>
+    <t>2025-11-29</t>
+  </si>
+  <si>
+    <t>SamsungElec</t>
+  </si>
+  <si>
+    <t>DB HiTek</t>
+  </si>
+  <si>
+    <t>SK hynix</t>
+  </si>
+  <si>
+    <t>240810.KS,0P00017YB3,330568</t>
   </si>
   <si>
     <t>058470.KS,0P0000ASU1,98886</t>
   </si>
   <si>
-    <t>SamsungElec</t>
-  </si>
-  <si>
-    <t>DB HiTek</t>
-  </si>
-  <si>
-    <t>SK hynix</t>
-  </si>
-  <si>
-    <t>240810.KS,0P00017YB3,330568</t>
-  </si>
-  <si>
     <t>403870.KS,0P0001PE9K,566428</t>
   </si>
   <si>
+    <t>005930.KS</t>
+  </si>
+  <si>
+    <t>000990.KS</t>
+  </si>
+  <si>
+    <t>000660.KS</t>
+  </si>
+  <si>
+    <t>240810.KS</t>
+  </si>
+  <si>
     <t>058470.KS</t>
   </si>
   <si>
-    <t>005930.KS</t>
-  </si>
-  <si>
-    <t>000990.KS</t>
-  </si>
-  <si>
-    <t>000660.KS</t>
-  </si>
-  <si>
-    <t>240810.KS</t>
-  </si>
-  <si>
     <t>403870.KS</t>
   </si>
   <si>
-    <t>건드리지 말기</t>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>📈 매수 관찰 구간입니다.</t>
+  </si>
+  <si>
+    <t>⛔ 관망하십시오.</t>
+  </si>
+  <si>
+    <t>🟢 완화적 (상승 우위)</t>
   </si>
 </sst>
 </file>
@@ -446,13 +467,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,200 +507,254 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>100500</v>
+      </c>
+      <c r="F2">
+        <v>6.01</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>63</v>
+      </c>
+      <c r="I2">
+        <v>73</v>
+      </c>
+      <c r="J2">
+        <v>73</v>
+      </c>
+      <c r="K2">
+        <v>60.8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2">
+        <v>85.36763896678245</v>
+      </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>63600</v>
+      </c>
+      <c r="F3">
+        <v>2.75</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>36</v>
+      </c>
+      <c r="I3">
+        <v>56</v>
+      </c>
+      <c r="J3">
+        <v>50</v>
+      </c>
+      <c r="K3">
+        <v>57</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3">
+        <v>85.36763896678245</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="D2">
-        <v>64500</v>
-      </c>
-      <c r="E2">
-        <v>62.5</v>
-      </c>
-      <c r="F2">
-        <v>14.97</v>
-      </c>
-      <c r="G2">
-        <v>50</v>
-      </c>
-      <c r="H2">
-        <v>50</v>
-      </c>
-      <c r="I2">
-        <v>43</v>
-      </c>
-      <c r="J2">
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>530000</v>
+      </c>
+      <c r="F4">
+        <v>1.8</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>60</v>
+      </c>
+      <c r="J4">
+        <v>70</v>
+      </c>
+      <c r="K4">
+        <v>55.6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4">
+        <v>85.36763896678245</v>
+      </c>
+      <c r="O4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>60300</v>
+      </c>
+      <c r="F5">
+        <v>-0.99</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>63</v>
       </c>
-      <c r="K2" t="s">
-        <v>24</v>
+      <c r="I5">
+        <v>56</v>
+      </c>
+      <c r="J5">
+        <v>63</v>
+      </c>
+      <c r="K5">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5">
+        <v>85.36763896678245</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>103500</v>
-      </c>
-      <c r="E3">
-        <v>57.4</v>
-      </c>
-      <c r="F3">
-        <v>2.88</v>
-      </c>
-      <c r="G3">
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>64800</v>
+      </c>
+      <c r="F6">
+        <v>11.53</v>
+      </c>
+      <c r="G6">
         <v>40</v>
       </c>
-      <c r="H3">
-        <v>56</v>
-      </c>
-      <c r="I3">
-        <v>70</v>
-      </c>
-      <c r="J3">
-        <v>80</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
+      <c r="H6">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>63</v>
+      </c>
+      <c r="K6">
+        <v>50.8</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <v>85.36763896678245</v>
+      </c>
+      <c r="O6" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>63600</v>
-      </c>
-      <c r="E4">
-        <v>63.1</v>
-      </c>
-      <c r="F4">
-        <v>-4.22</v>
-      </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="H4">
-        <v>53</v>
-      </c>
-      <c r="I4">
-        <v>53</v>
-      </c>
-      <c r="J4">
-        <v>53</v>
-      </c>
-      <c r="K4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="D5">
-        <v>544000</v>
-      </c>
-      <c r="E5">
-        <v>43.5</v>
-      </c>
-      <c r="F5">
-        <v>-4.66</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
-        <v>73</v>
-      </c>
-      <c r="I5">
-        <v>60</v>
-      </c>
-      <c r="J5">
-        <v>76</v>
-      </c>
-      <c r="K5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>61300</v>
-      </c>
-      <c r="E6">
-        <v>32.1</v>
-      </c>
-      <c r="F6">
-        <v>0.33</v>
-      </c>
-      <c r="G6">
-        <v>20</v>
-      </c>
-      <c r="H6">
-        <v>56</v>
-      </c>
-      <c r="I6">
-        <v>60</v>
-      </c>
-      <c r="J6">
-        <v>60</v>
-      </c>
-      <c r="K6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>28800</v>
       </c>
-      <c r="E7">
-        <v>31.9</v>
-      </c>
       <c r="F7">
-        <v>-0.86</v>
+        <v>-4.48</v>
       </c>
       <c r="G7">
         <v>10</v>
@@ -688,13 +763,25 @@
         <v>40</v>
       </c>
       <c r="I7">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="J7">
-        <v>50</v>
-      </c>
-      <c r="K7" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <v>44.6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7">
+        <v>85.36763896678245</v>
+      </c>
+      <c r="O7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 03:23:53
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -549,7 +549,7 @@
         <v>73</v>
       </c>
       <c r="K2">
-        <v>60.8</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.36763896678245</v>
+        <v>85.96878041621773</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -593,7 +593,7 @@
         <v>50</v>
       </c>
       <c r="K3">
-        <v>57</v>
+        <v>57.2</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.36763896678245</v>
+        <v>85.96878041621773</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -637,7 +637,7 @@
         <v>70</v>
       </c>
       <c r="K4">
-        <v>55.6</v>
+        <v>55.8</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.36763896678245</v>
+        <v>85.96878041621773</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -681,7 +681,7 @@
         <v>63</v>
       </c>
       <c r="K5">
-        <v>51</v>
+        <v>51.2</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.36763896678245</v>
+        <v>85.96878041621773</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -725,7 +725,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>50.8</v>
+        <v>51</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.36763896678245</v>
+        <v>85.96878041621773</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -769,7 +769,7 @@
         <v>53</v>
       </c>
       <c r="K7">
-        <v>44.6</v>
+        <v>44.8</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.36763896678245</v>
+        <v>85.96878041621773</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 03:44:01
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.96878041621773</v>
+        <v>85.83574689470727</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.96878041621773</v>
+        <v>85.83574689470727</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.96878041621773</v>
+        <v>85.83574689470727</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.96878041621773</v>
+        <v>85.83574689470727</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.96878041621773</v>
+        <v>85.83574689470727</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.96878041621773</v>
+        <v>85.83574689470727</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 03:48:30
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -549,7 +549,7 @@
         <v>73</v>
       </c>
       <c r="K2">
-        <v>61</v>
+        <v>60.9</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.83574689470727</v>
+        <v>85.82376350509293</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -593,7 +593,7 @@
         <v>50</v>
       </c>
       <c r="K3">
-        <v>57.2</v>
+        <v>57.1</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.83574689470727</v>
+        <v>85.82376350509293</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -637,7 +637,7 @@
         <v>70</v>
       </c>
       <c r="K4">
-        <v>55.8</v>
+        <v>55.7</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.83574689470727</v>
+        <v>85.82376350509293</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -681,7 +681,7 @@
         <v>63</v>
       </c>
       <c r="K5">
-        <v>51.2</v>
+        <v>51.1</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.83574689470727</v>
+        <v>85.82376350509293</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -725,7 +725,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>51</v>
+        <v>50.9</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.83574689470727</v>
+        <v>85.82376350509293</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -769,7 +769,7 @@
         <v>53</v>
       </c>
       <c r="K7">
-        <v>44.8</v>
+        <v>44.7</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.83574689470727</v>
+        <v>85.82376350509293</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 03:52:35
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.82376350509293</v>
+        <v>85.77505782882612</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.82376350509293</v>
+        <v>85.77505782882612</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.82376350509293</v>
+        <v>85.77505782882612</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.82376350509293</v>
+        <v>85.77505782882612</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.82376350509293</v>
+        <v>85.77505782882612</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.82376350509293</v>
+        <v>85.77505782882612</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 04:04:56
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -549,7 +549,7 @@
         <v>73</v>
       </c>
       <c r="K2">
-        <v>60.9</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.77505782882612</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -593,7 +593,7 @@
         <v>50</v>
       </c>
       <c r="K3">
-        <v>57.1</v>
+        <v>57.2</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.77505782882612</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -637,7 +637,7 @@
         <v>70</v>
       </c>
       <c r="K4">
-        <v>55.7</v>
+        <v>55.8</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.77505782882612</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -681,7 +681,7 @@
         <v>63</v>
       </c>
       <c r="K5">
-        <v>51.1</v>
+        <v>51.2</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.77505782882612</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -725,7 +725,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>50.9</v>
+        <v>51</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.77505782882612</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -769,7 +769,7 @@
         <v>53</v>
       </c>
       <c r="K7">
-        <v>44.7</v>
+        <v>44.8</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.77505782882612</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 04:16:23
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.8724807945396</v>
+        <v>85.92117485762657</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.8724807945396</v>
+        <v>85.92117485762657</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.8724807945396</v>
+        <v>85.92117485762657</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.8724807945396</v>
+        <v>85.92117485762657</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.8724807945396</v>
+        <v>85.92117485762657</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.8724807945396</v>
+        <v>85.92117485762657</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 04:59:05
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -67,34 +67,34 @@
     <t>SamsungElec</t>
   </si>
   <si>
+    <t>240810.KS,0P00017YB3,330568</t>
+  </si>
+  <si>
+    <t>058470.KS,0P0000ASU1,98886</t>
+  </si>
+  <si>
     <t>DB HiTek</t>
   </si>
   <si>
     <t>SK hynix</t>
   </si>
   <si>
-    <t>240810.KS,0P00017YB3,330568</t>
-  </si>
-  <si>
-    <t>058470.KS,0P0000ASU1,98886</t>
-  </si>
-  <si>
     <t>403870.KS,0P0001PE9K,566428</t>
   </si>
   <si>
     <t>005930.KS</t>
   </si>
   <si>
+    <t>240810.KS</t>
+  </si>
+  <si>
+    <t>058470.KS</t>
+  </si>
+  <si>
     <t>000990.KS</t>
   </si>
   <si>
     <t>000660.KS</t>
-  </si>
-  <si>
-    <t>240810.KS</t>
-  </si>
-  <si>
-    <t>058470.KS</t>
   </si>
   <si>
     <t>403870.KS</t>
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.92117485762657</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -575,25 +575,25 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>63600</v>
+        <v>61300</v>
       </c>
       <c r="F3">
-        <v>2.75</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H3">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="I3">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="K3">
-        <v>57.2</v>
+        <v>59.8</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -602,7 +602,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.92117485762657</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -619,25 +619,25 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>530000</v>
+        <v>68300</v>
       </c>
       <c r="F4">
-        <v>1.8</v>
+        <v>25.55</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H4">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="I4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J4">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="K4">
-        <v>55.8</v>
+        <v>57.8</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -646,7 +646,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.92117485762657</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -663,25 +663,25 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>60300</v>
+        <v>63600</v>
       </c>
       <c r="F5">
-        <v>-0.99</v>
+        <v>2.75</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H5">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="I5">
         <v>56</v>
       </c>
       <c r="J5">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="K5">
-        <v>51.2</v>
+        <v>57.2</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -690,7 +690,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.92117485762657</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -707,25 +707,25 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>64800</v>
+        <v>530000</v>
       </c>
       <c r="F6">
-        <v>11.53</v>
+        <v>1.8</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H6">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="I6">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="J6">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="K6">
-        <v>51</v>
+        <v>55.8</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -734,7 +734,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.92117485762657</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -751,25 +751,25 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>28800</v>
+        <v>30250</v>
       </c>
       <c r="F7">
-        <v>-4.48</v>
+        <v>6.7</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H7">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I7">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="J7">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K7">
-        <v>44.8</v>
+        <v>50.2</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.92117485762657</v>
+        <v>85.8724807945396</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-29 18:42:09
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -67,15 +67,15 @@
     <t>SamsungElec</t>
   </si>
   <si>
+    <t>DB HiTek</t>
+  </si>
+  <si>
     <t>240810.KS,0P00017YB3,330568</t>
   </si>
   <si>
     <t>058470.KS,0P0000ASU1,98886</t>
   </si>
   <si>
-    <t>DB HiTek</t>
-  </si>
-  <si>
     <t>SK hynix</t>
   </si>
   <si>
@@ -85,13 +85,13 @@
     <t>005930.KS</t>
   </si>
   <si>
+    <t>000990.KS</t>
+  </si>
+  <si>
     <t>240810.KS</t>
   </si>
   <si>
     <t>058470.KS</t>
-  </si>
-  <si>
-    <t>000990.KS</t>
   </si>
   <si>
     <t>000660.KS</t>
@@ -533,11 +533,14 @@
       <c r="D2">
         <v>100500</v>
       </c>
+      <c r="E2">
+        <v>49.9</v>
+      </c>
       <c r="F2">
         <v>6.01</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H2">
         <v>63</v>
@@ -549,7 +552,7 @@
         <v>73</v>
       </c>
       <c r="K2">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -558,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.8724807945396</v>
+        <v>85.87127175646313</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -575,34 +578,37 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>61300</v>
+        <v>63600</v>
+      </c>
+      <c r="E3">
+        <v>53</v>
       </c>
       <c r="F3">
-        <v>8.109999999999999</v>
+        <v>2.75</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H3">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="I3">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="J3">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="K3">
-        <v>59.8</v>
+        <v>60.2</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N3">
-        <v>85.8724807945396</v>
+        <v>85.87127175646313</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -619,25 +625,28 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>68300</v>
+        <v>61300</v>
+      </c>
+      <c r="E4">
+        <v>30.8</v>
       </c>
       <c r="F4">
-        <v>25.55</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H4">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="J4">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K4">
-        <v>57.8</v>
+        <v>59.8</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -646,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.8724807945396</v>
+        <v>85.87127175646313</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -663,25 +672,28 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>63600</v>
+        <v>68300</v>
+      </c>
+      <c r="E5">
+        <v>71.40000000000001</v>
       </c>
       <c r="F5">
-        <v>2.75</v>
+        <v>25.55</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H5">
         <v>36</v>
       </c>
       <c r="I5">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="J5">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="K5">
-        <v>57.2</v>
+        <v>57.8</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -690,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.8724807945396</v>
+        <v>85.87127175646313</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -709,6 +721,9 @@
       <c r="D6">
         <v>530000</v>
       </c>
+      <c r="E6">
+        <v>35.6</v>
+      </c>
       <c r="F6">
         <v>1.8</v>
       </c>
@@ -734,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.8724807945396</v>
+        <v>85.87127175646313</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -753,6 +768,9 @@
       <c r="D7">
         <v>30250</v>
       </c>
+      <c r="E7">
+        <v>39.7</v>
+      </c>
       <c r="F7">
         <v>6.7</v>
       </c>
@@ -778,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.8724807945396</v>
+        <v>85.87127175646313</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-01 01:09:22
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -61,7 +61,7 @@
     <t>MACRO_SIGNAL</t>
   </si>
   <si>
-    <t>2025-11-29</t>
+    <t>2025-12-01</t>
   </si>
   <si>
     <t>SamsungElec</t>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.87127175646313</v>
+        <v>85.87246918135976</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -608,7 +608,7 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>85.87127175646313</v>
+        <v>85.87246918135976</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.87127175646313</v>
+        <v>85.87246918135976</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.87127175646313</v>
+        <v>85.87246918135976</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.87127175646313</v>
+        <v>85.87246918135976</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.87127175646313</v>
+        <v>85.87246918135976</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-01 14:08:26
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -67,34 +67,34 @@
     <t>SamsungElec</t>
   </si>
   <si>
+    <t>240810.KS,0P00017YB3,330568</t>
+  </si>
+  <si>
     <t>DB HiTek</t>
   </si>
   <si>
-    <t>240810.KS,0P00017YB3,330568</t>
+    <t>SK hynix</t>
   </si>
   <si>
     <t>058470.KS,0P0000ASU1,98886</t>
   </si>
   <si>
-    <t>SK hynix</t>
-  </si>
-  <si>
     <t>403870.KS,0P0001PE9K,566428</t>
   </si>
   <si>
     <t>005930.KS</t>
   </si>
   <si>
+    <t>240810.KS</t>
+  </si>
+  <si>
     <t>000990.KS</t>
   </si>
   <si>
-    <t>240810.KS</t>
+    <t>000660.KS</t>
   </si>
   <si>
     <t>058470.KS</t>
-  </si>
-  <si>
-    <t>000660.KS</t>
   </si>
   <si>
     <t>403870.KS</t>
@@ -531,28 +531,28 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>100500</v>
+        <v>101100</v>
       </c>
       <c r="E2">
-        <v>49.9</v>
+        <v>46.7</v>
       </c>
       <c r="F2">
-        <v>6.01</v>
+        <v>4.55</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H2">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I2">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J2">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="K2">
-        <v>64</v>
+        <v>68.8</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.87246918135976</v>
+        <v>85.92500513438651</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,37 +578,37 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>63600</v>
+        <v>61300</v>
       </c>
       <c r="E3">
-        <v>53</v>
+        <v>30.8</v>
       </c>
       <c r="F3">
-        <v>2.75</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="G3">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H3">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="I3">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="J3">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="K3">
-        <v>60.2</v>
+        <v>59.8</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N3">
-        <v>85.87246918135976</v>
+        <v>85.92500513438651</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -625,28 +625,28 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>61300</v>
+        <v>65100</v>
       </c>
       <c r="E4">
-        <v>30.8</v>
+        <v>41.9</v>
       </c>
       <c r="F4">
-        <v>8.109999999999999</v>
+        <v>7.07</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H4">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="I4">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="J4">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K4">
-        <v>59.8</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.87246918135976</v>
+        <v>85.92500513438651</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,28 +672,28 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>68300</v>
+        <v>544000</v>
       </c>
       <c r="E5">
-        <v>71.40000000000001</v>
+        <v>35.8</v>
       </c>
       <c r="F5">
-        <v>25.55</v>
+        <v>4.69</v>
       </c>
       <c r="G5">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="I5">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="J5">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="K5">
-        <v>57.8</v>
+        <v>58.2</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.87246918135976</v>
+        <v>85.92500513438651</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -719,28 +719,28 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>530000</v>
+        <v>68300</v>
       </c>
       <c r="E6">
-        <v>35.6</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="F6">
-        <v>1.8</v>
+        <v>25.55</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H6">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="I6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J6">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K6">
-        <v>55.8</v>
+        <v>57.8</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.87246918135976</v>
+        <v>85.92500513438651</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.87246918135976</v>
+        <v>85.92500513438651</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-03 03:05:24
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -61,45 +61,45 @@
     <t>MACRO_SIGNAL</t>
   </si>
   <si>
-    <t>2025-12-01</t>
+    <t>2025-12-03</t>
+  </si>
+  <si>
+    <t>058470.KS,0P0000ASU1,98886</t>
   </si>
   <si>
     <t>SamsungElec</t>
   </si>
   <si>
+    <t>403870.KS,0P0001PE9K,566428</t>
+  </si>
+  <si>
+    <t>DB HiTek</t>
+  </si>
+  <si>
+    <t>SK hynix</t>
+  </si>
+  <si>
     <t>240810.KS,0P00017YB3,330568</t>
   </si>
   <si>
-    <t>DB HiTek</t>
-  </si>
-  <si>
-    <t>SK hynix</t>
-  </si>
-  <si>
-    <t>058470.KS,0P0000ASU1,98886</t>
-  </si>
-  <si>
-    <t>403870.KS,0P0001PE9K,566428</t>
+    <t>058470.KS</t>
   </si>
   <si>
     <t>005930.KS</t>
   </si>
   <si>
+    <t>403870.KS</t>
+  </si>
+  <si>
+    <t>000990.KS</t>
+  </si>
+  <si>
+    <t>000660.KS</t>
+  </si>
+  <si>
     <t>240810.KS</t>
   </si>
   <si>
-    <t>000990.KS</t>
-  </si>
-  <si>
-    <t>000660.KS</t>
-  </si>
-  <si>
-    <t>058470.KS</t>
-  </si>
-  <si>
-    <t>403870.KS</t>
-  </si>
-  <si>
     <t>Pattern</t>
   </si>
   <si>
@@ -109,7 +109,7 @@
     <t>⛔ 관망하십시오.</t>
   </si>
   <si>
-    <t>🟢 완화적 (상승 우위)</t>
+    <t>🟢 상승 우위 (다소 완화)</t>
   </si>
 </sst>
 </file>
@@ -531,28 +531,28 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>101100</v>
+        <v>66600</v>
       </c>
       <c r="E2">
-        <v>46.7</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="F2">
-        <v>4.55</v>
+        <v>18.09</v>
       </c>
       <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2">
         <v>50</v>
       </c>
-      <c r="H2">
+      <c r="I2">
+        <v>63</v>
+      </c>
+      <c r="J2">
         <v>70</v>
       </c>
-      <c r="I2">
-        <v>70</v>
-      </c>
-      <c r="J2">
-        <v>83</v>
-      </c>
       <c r="K2">
-        <v>68.8</v>
+        <v>62.8</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>85.92500513438651</v>
+        <v>65.32892478746797</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,28 +578,28 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>61300</v>
+        <v>103400</v>
       </c>
       <c r="E3">
-        <v>30.8</v>
+        <v>50.4</v>
       </c>
       <c r="F3">
-        <v>8.109999999999999</v>
+        <v>4.13</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <v>63</v>
       </c>
       <c r="I3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J3">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="K3">
-        <v>59.8</v>
+        <v>58.6</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>85.92500513438651</v>
+        <v>65.32892478746797</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -625,16 +625,16 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>65100</v>
+        <v>31300</v>
       </c>
       <c r="E4">
-        <v>41.9</v>
+        <v>46.2</v>
       </c>
       <c r="F4">
-        <v>7.07</v>
+        <v>10.99</v>
       </c>
       <c r="G4">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H4">
         <v>43</v>
@@ -646,7 +646,7 @@
         <v>60</v>
       </c>
       <c r="K4">
-        <v>59</v>
+        <v>55.8</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>85.92500513438651</v>
+        <v>65.32892478746797</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,28 +672,28 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>544000</v>
+        <v>65000</v>
       </c>
       <c r="E5">
-        <v>35.8</v>
+        <v>35.3</v>
       </c>
       <c r="F5">
-        <v>4.69</v>
+        <v>5.01</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H5">
         <v>53</v>
       </c>
       <c r="I5">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J5">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="K5">
-        <v>58.2</v>
+        <v>52.6</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>85.92500513438651</v>
+        <v>65.32892478746797</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -719,28 +719,28 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>68300</v>
+        <v>558000</v>
       </c>
       <c r="E6">
-        <v>71.40000000000001</v>
+        <v>39.4</v>
       </c>
       <c r="F6">
-        <v>25.55</v>
+        <v>7.59</v>
       </c>
       <c r="G6">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H6">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="I6">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="J6">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="K6">
-        <v>57.8</v>
+        <v>50.8</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>85.92500513438651</v>
+        <v>65.32892478746797</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -766,28 +766,28 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>30250</v>
+        <v>61500</v>
       </c>
       <c r="E7">
-        <v>39.7</v>
+        <v>28.6</v>
       </c>
       <c r="F7">
-        <v>6.7</v>
+        <v>3.71</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="I7">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="J7">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="K7">
-        <v>50.2</v>
+        <v>49.6</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>85.92500513438651</v>
+        <v>65.32892478746797</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-03 08:54:10
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -531,28 +531,28 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>66600</v>
+        <v>65600</v>
       </c>
       <c r="E2">
-        <v>66.90000000000001</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="F2">
-        <v>18.09</v>
+        <v>3.96</v>
       </c>
       <c r="G2">
         <v>60</v>
       </c>
       <c r="H2">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I2">
+        <v>56</v>
+      </c>
+      <c r="J2">
         <v>63</v>
       </c>
-      <c r="J2">
-        <v>70</v>
-      </c>
       <c r="K2">
-        <v>62.8</v>
+        <v>60.2</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>65.32892478746797</v>
+        <v>66.04328690552585</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>58.6</v>
+        <v>58.8</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>65.32892478746797</v>
+        <v>66.04328690552585</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -625,28 +625,28 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>31300</v>
+        <v>31250</v>
       </c>
       <c r="E4">
-        <v>46.2</v>
+        <v>43.9</v>
       </c>
       <c r="F4">
-        <v>10.99</v>
+        <v>10.62</v>
       </c>
       <c r="G4">
         <v>50</v>
       </c>
       <c r="H4">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I4">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J4">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K4">
-        <v>55.8</v>
+        <v>54.8</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>65.32892478746797</v>
+        <v>66.04328690552585</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -693,7 +693,7 @@
         <v>60</v>
       </c>
       <c r="K5">
-        <v>52.6</v>
+        <v>52.8</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>65.32892478746797</v>
+        <v>66.04328690552585</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>73</v>
       </c>
       <c r="K6">
-        <v>50.8</v>
+        <v>51</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>65.32892478746797</v>
+        <v>66.04328690552585</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -766,28 +766,28 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>61500</v>
+        <v>61700</v>
       </c>
       <c r="E7">
-        <v>28.6</v>
+        <v>30.2</v>
       </c>
       <c r="F7">
-        <v>3.71</v>
+        <v>2.83</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
         <v>63</v>
       </c>
-      <c r="I7">
-        <v>60</v>
-      </c>
       <c r="J7">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="K7">
-        <v>49.6</v>
+        <v>51</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>65.32892478746797</v>
+        <v>66.04328690552585</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-03 09:03:30
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -590,22 +590,22 @@
         <v>50</v>
       </c>
       <c r="H3">
+        <v>66</v>
+      </c>
+      <c r="I3">
         <v>63</v>
       </c>
-      <c r="I3">
+      <c r="J3">
+        <v>80</v>
+      </c>
+      <c r="K3">
         <v>60</v>
-      </c>
-      <c r="J3">
-        <v>76</v>
-      </c>
-      <c r="K3">
-        <v>58.8</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N3">
         <v>66.04328690552585</v>
@@ -731,16 +731,16 @@
         <v>20</v>
       </c>
       <c r="H6">
+        <v>70</v>
+      </c>
+      <c r="I6">
         <v>66</v>
-      </c>
-      <c r="I6">
-        <v>63</v>
       </c>
       <c r="J6">
         <v>73</v>
       </c>
       <c r="K6">
-        <v>51</v>
+        <v>52.2</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-03 10:00:39
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -64,37 +64,37 @@
     <t>2025-12-03</t>
   </si>
   <si>
+    <t>DB HiTek</t>
+  </si>
+  <si>
+    <t>SamsungElec</t>
+  </si>
+  <si>
     <t>058470.KS,0P0000ASU1,98886</t>
   </si>
   <si>
-    <t>SamsungElec</t>
+    <t>SK hynix</t>
   </si>
   <si>
     <t>403870.KS,0P0001PE9K,566428</t>
   </si>
   <si>
-    <t>DB HiTek</t>
-  </si>
-  <si>
-    <t>SK hynix</t>
-  </si>
-  <si>
     <t>240810.KS,0P00017YB3,330568</t>
   </si>
   <si>
+    <t>000990.KS</t>
+  </si>
+  <si>
+    <t>005930.KS</t>
+  </si>
+  <si>
     <t>058470.KS</t>
   </si>
   <si>
-    <t>005930.KS</t>
+    <t>000660.KS</t>
   </si>
   <si>
     <t>403870.KS</t>
-  </si>
-  <si>
-    <t>000990.KS</t>
-  </si>
-  <si>
-    <t>000660.KS</t>
   </si>
   <si>
     <t>240810.KS</t>
@@ -531,28 +531,28 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>65600</v>
+        <v>64800</v>
       </c>
       <c r="E2">
-        <v>65.09999999999999</v>
+        <v>42.6</v>
       </c>
       <c r="F2">
-        <v>3.96</v>
+        <v>4.68</v>
       </c>
       <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
         <v>60</v>
       </c>
-      <c r="H2">
-        <v>46</v>
-      </c>
       <c r="I2">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="J2">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="K2">
-        <v>60.2</v>
+        <v>62.8</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>66.04328690552585</v>
+        <v>66.09241856096124</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,28 +578,28 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>103400</v>
+        <v>104800</v>
       </c>
       <c r="E3">
-        <v>50.4</v>
+        <v>52.6</v>
       </c>
       <c r="F3">
-        <v>4.13</v>
+        <v>1.95</v>
       </c>
       <c r="G3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H3">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="I3">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="J3">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="K3">
-        <v>60</v>
+        <v>60.2</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>66.04328690552585</v>
+        <v>66.09241856096124</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -625,37 +625,37 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>31250</v>
+        <v>65600</v>
       </c>
       <c r="E4">
-        <v>43.9</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="F4">
-        <v>10.62</v>
+        <v>3.96</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H4">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I4">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J4">
         <v>63</v>
       </c>
       <c r="K4">
-        <v>54.8</v>
+        <v>60.2</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N4">
-        <v>66.04328690552585</v>
+        <v>66.09241856096124</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,28 +672,28 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>65000</v>
+        <v>548500</v>
       </c>
       <c r="E5">
-        <v>35.3</v>
+        <v>38.7</v>
       </c>
       <c r="F5">
-        <v>5.01</v>
+        <v>4.75</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="I5">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="J5">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K5">
-        <v>52.8</v>
+        <v>56.2</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>66.04328690552585</v>
+        <v>66.09241856096124</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -719,28 +719,28 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>558000</v>
+        <v>31250</v>
       </c>
       <c r="E6">
-        <v>39.4</v>
+        <v>43.9</v>
       </c>
       <c r="F6">
-        <v>7.59</v>
+        <v>10.62</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H6">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="I6">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="J6">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="K6">
-        <v>52.2</v>
+        <v>54.8</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>66.04328690552585</v>
+        <v>66.09241856096124</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>66.04328690552585</v>
+        <v>66.09241856096124</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 02:00:49
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>날짜</t>
   </si>
@@ -61,55 +61,52 @@
     <t>MACRO_SIGNAL</t>
   </si>
   <si>
-    <t>2025-12-03</t>
+    <t>2025-12-05</t>
+  </si>
+  <si>
+    <t>SamsungElec</t>
+  </si>
+  <si>
+    <t>058470.KS,0P0000ASU1,98886</t>
+  </si>
+  <si>
+    <t>403870.KS,0P0001PE9K,566428</t>
+  </si>
+  <si>
+    <t>SK hynix</t>
   </si>
   <si>
     <t>DB HiTek</t>
   </si>
   <si>
-    <t>SamsungElec</t>
-  </si>
-  <si>
-    <t>058470.KS,0P0000ASU1,98886</t>
-  </si>
-  <si>
-    <t>SK hynix</t>
-  </si>
-  <si>
-    <t>403870.KS,0P0001PE9K,566428</t>
-  </si>
-  <si>
     <t>240810.KS,0P00017YB3,330568</t>
   </si>
   <si>
+    <t>005930.KS</t>
+  </si>
+  <si>
+    <t>058470.KS</t>
+  </si>
+  <si>
+    <t>403870.KS</t>
+  </si>
+  <si>
+    <t>000660.KS</t>
+  </si>
+  <si>
     <t>000990.KS</t>
   </si>
   <si>
-    <t>005930.KS</t>
-  </si>
-  <si>
-    <t>058470.KS</t>
-  </si>
-  <si>
-    <t>000660.KS</t>
-  </si>
-  <si>
-    <t>403870.KS</t>
-  </si>
-  <si>
     <t>240810.KS</t>
   </si>
   <si>
     <t>Pattern</t>
   </si>
   <si>
-    <t>📈 매수 관찰 구간입니다.</t>
-  </si>
-  <si>
     <t>⛔ 관망하십시오.</t>
   </si>
   <si>
-    <t>🟢 상승 우위 (다소 완화)</t>
+    <t>⚪ 중립 구간</t>
   </si>
 </sst>
 </file>
@@ -531,28 +528,28 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>64800</v>
+        <v>105100</v>
       </c>
       <c r="E2">
-        <v>42.6</v>
+        <v>61.7</v>
       </c>
       <c r="F2">
-        <v>4.68</v>
+        <v>1.55</v>
       </c>
       <c r="G2">
+        <v>60</v>
+      </c>
+      <c r="H2">
         <v>50</v>
       </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
       <c r="I2">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="K2">
-        <v>62.8</v>
+        <v>56.1</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,10 +558,10 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>66.09241856096124</v>
+        <v>52.43913937059539</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -578,28 +575,28 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>104800</v>
+        <v>66000</v>
       </c>
       <c r="E3">
-        <v>52.6</v>
+        <v>67.09999999999999</v>
       </c>
       <c r="F3">
-        <v>1.95</v>
+        <v>2.33</v>
       </c>
       <c r="G3">
         <v>60</v>
       </c>
       <c r="H3">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I3">
         <v>56</v>
       </c>
       <c r="J3">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K3">
-        <v>60.2</v>
+        <v>56.1</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,10 +605,10 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>66.09241856096124</v>
+        <v>52.43913937059539</v>
       </c>
       <c r="O3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -625,28 +622,28 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>65600</v>
+        <v>31000</v>
       </c>
       <c r="E4">
-        <v>65.09999999999999</v>
+        <v>41.2</v>
       </c>
       <c r="F4">
-        <v>3.96</v>
+        <v>7.64</v>
       </c>
       <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>50</v>
+      </c>
+      <c r="I4">
+        <v>53</v>
+      </c>
+      <c r="J4">
         <v>60</v>
       </c>
-      <c r="H4">
-        <v>46</v>
-      </c>
-      <c r="I4">
-        <v>56</v>
-      </c>
-      <c r="J4">
-        <v>63</v>
-      </c>
       <c r="K4">
-        <v>60.2</v>
+        <v>51.9</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,10 +652,10 @@
         <v>29</v>
       </c>
       <c r="N4">
-        <v>66.09241856096124</v>
+        <v>52.43913937059539</v>
       </c>
       <c r="O4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -672,40 +669,40 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>548500</v>
+        <v>542000</v>
       </c>
       <c r="E5">
-        <v>38.7</v>
+        <v>46.2</v>
       </c>
       <c r="F5">
-        <v>4.75</v>
+        <v>-0.37</v>
       </c>
       <c r="G5">
         <v>20</v>
       </c>
       <c r="H5">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I5">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="J5">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="K5">
-        <v>56.2</v>
+        <v>46.9</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
       </c>
       <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5">
+        <v>52.43913937059539</v>
+      </c>
+      <c r="O5" t="s">
         <v>30</v>
-      </c>
-      <c r="N5">
-        <v>66.09241856096124</v>
-      </c>
-      <c r="O5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -719,40 +716,40 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>31250</v>
+        <v>64400</v>
       </c>
       <c r="E6">
-        <v>43.9</v>
+        <v>41.9</v>
       </c>
       <c r="F6">
-        <v>10.62</v>
+        <v>1.26</v>
       </c>
       <c r="G6">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H6">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I6">
         <v>50</v>
       </c>
       <c r="J6">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="K6">
-        <v>54.8</v>
+        <v>44.7</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
       </c>
       <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6">
+        <v>52.43913937059539</v>
+      </c>
+      <c r="O6" t="s">
         <v>30</v>
-      </c>
-      <c r="N6">
-        <v>66.09241856096124</v>
-      </c>
-      <c r="O6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -766,40 +763,40 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>61700</v>
+        <v>61900</v>
       </c>
       <c r="E7">
-        <v>30.2</v>
+        <v>32.5</v>
       </c>
       <c r="F7">
-        <v>2.83</v>
+        <v>0.98</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="I7">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="J7">
         <v>56</v>
       </c>
       <c r="K7">
-        <v>51</v>
+        <v>44.1</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
       </c>
       <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7">
+        <v>52.43913937059539</v>
+      </c>
+      <c r="O7" t="s">
         <v>30</v>
-      </c>
-      <c r="N7">
-        <v>66.09241856096124</v>
-      </c>
-      <c r="O7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 02:03:00
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>52.43913937059539</v>
+        <v>52.47848103381103</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
@@ -605,7 +605,7 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>52.43913937059539</v>
+        <v>52.47848103381103</v>
       </c>
       <c r="O3" t="s">
         <v>30</v>
@@ -652,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="N4">
-        <v>52.43913937059539</v>
+        <v>52.47848103381103</v>
       </c>
       <c r="O4" t="s">
         <v>30</v>
@@ -699,7 +699,7 @@
         <v>29</v>
       </c>
       <c r="N5">
-        <v>52.43913937059539</v>
+        <v>52.47848103381103</v>
       </c>
       <c r="O5" t="s">
         <v>30</v>
@@ -746,7 +746,7 @@
         <v>29</v>
       </c>
       <c r="N6">
-        <v>52.43913937059539</v>
+        <v>52.47848103381103</v>
       </c>
       <c r="O6" t="s">
         <v>30</v>
@@ -793,7 +793,7 @@
         <v>29</v>
       </c>
       <c r="N7">
-        <v>52.43913937059539</v>
+        <v>52.47848103381103</v>
       </c>
       <c r="O7" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 02:39:10
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -549,7 +549,7 @@
         <v>73</v>
       </c>
       <c r="K2">
-        <v>56.1</v>
+        <v>56.5</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>52.47848103381103</v>
+        <v>53.62998959737769</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
@@ -596,7 +596,7 @@
         <v>66</v>
       </c>
       <c r="K3">
-        <v>56.1</v>
+        <v>56.5</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -605,7 +605,7 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>52.47848103381103</v>
+        <v>53.62998959737769</v>
       </c>
       <c r="O3" t="s">
         <v>30</v>
@@ -643,7 +643,7 @@
         <v>60</v>
       </c>
       <c r="K4">
-        <v>51.9</v>
+        <v>52.3</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -652,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="N4">
-        <v>52.47848103381103</v>
+        <v>53.62998959737769</v>
       </c>
       <c r="O4" t="s">
         <v>30</v>
@@ -690,7 +690,7 @@
         <v>70</v>
       </c>
       <c r="K5">
-        <v>46.9</v>
+        <v>47.3</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -699,7 +699,7 @@
         <v>29</v>
       </c>
       <c r="N5">
-        <v>52.47848103381103</v>
+        <v>53.62998959737769</v>
       </c>
       <c r="O5" t="s">
         <v>30</v>
@@ -737,7 +737,7 @@
         <v>50</v>
       </c>
       <c r="K6">
-        <v>44.7</v>
+        <v>45.1</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -746,7 +746,7 @@
         <v>29</v>
       </c>
       <c r="N6">
-        <v>52.47848103381103</v>
+        <v>53.62998959737769</v>
       </c>
       <c r="O6" t="s">
         <v>30</v>
@@ -784,7 +784,7 @@
         <v>56</v>
       </c>
       <c r="K7">
-        <v>44.1</v>
+        <v>44.5</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -793,7 +793,7 @@
         <v>29</v>
       </c>
       <c r="N7">
-        <v>52.47848103381103</v>
+        <v>53.62998959737769</v>
       </c>
       <c r="O7" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 03:03:39
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>53.62998959737769</v>
+        <v>53.71147335634279</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
@@ -605,7 +605,7 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>53.62998959737769</v>
+        <v>53.71147335634279</v>
       </c>
       <c r="O3" t="s">
         <v>30</v>
@@ -652,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="N4">
-        <v>53.62998959737769</v>
+        <v>53.71147335634279</v>
       </c>
       <c r="O4" t="s">
         <v>30</v>
@@ -699,7 +699,7 @@
         <v>29</v>
       </c>
       <c r="N5">
-        <v>53.62998959737769</v>
+        <v>53.71147335634279</v>
       </c>
       <c r="O5" t="s">
         <v>30</v>
@@ -746,7 +746,7 @@
         <v>29</v>
       </c>
       <c r="N6">
-        <v>53.62998959737769</v>
+        <v>53.71147335634279</v>
       </c>
       <c r="O6" t="s">
         <v>30</v>
@@ -793,7 +793,7 @@
         <v>29</v>
       </c>
       <c r="N7">
-        <v>53.62998959737769</v>
+        <v>53.71147335634279</v>
       </c>
       <c r="O7" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 04:00:45
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -549,7 +549,7 @@
         <v>73</v>
       </c>
       <c r="K2">
-        <v>56.5</v>
+        <v>56.6</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -558,7 +558,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>53.71147335634279</v>
+        <v>54.02451352198364</v>
       </c>
       <c r="O2" t="s">
         <v>30</v>
@@ -596,7 +596,7 @@
         <v>66</v>
       </c>
       <c r="K3">
-        <v>56.5</v>
+        <v>56.6</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -605,7 +605,7 @@
         <v>29</v>
       </c>
       <c r="N3">
-        <v>53.71147335634279</v>
+        <v>54.02451352198364</v>
       </c>
       <c r="O3" t="s">
         <v>30</v>
@@ -643,7 +643,7 @@
         <v>60</v>
       </c>
       <c r="K4">
-        <v>52.3</v>
+        <v>52.4</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -652,7 +652,7 @@
         <v>29</v>
       </c>
       <c r="N4">
-        <v>53.71147335634279</v>
+        <v>54.02451352198364</v>
       </c>
       <c r="O4" t="s">
         <v>30</v>
@@ -690,7 +690,7 @@
         <v>70</v>
       </c>
       <c r="K5">
-        <v>47.3</v>
+        <v>47.4</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -699,7 +699,7 @@
         <v>29</v>
       </c>
       <c r="N5">
-        <v>53.71147335634279</v>
+        <v>54.02451352198364</v>
       </c>
       <c r="O5" t="s">
         <v>30</v>
@@ -737,7 +737,7 @@
         <v>50</v>
       </c>
       <c r="K6">
-        <v>45.1</v>
+        <v>45.2</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -746,7 +746,7 @@
         <v>29</v>
       </c>
       <c r="N6">
-        <v>53.71147335634279</v>
+        <v>54.02451352198364</v>
       </c>
       <c r="O6" t="s">
         <v>30</v>
@@ -784,7 +784,7 @@
         <v>56</v>
       </c>
       <c r="K7">
-        <v>44.5</v>
+        <v>44.6</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -793,7 +793,7 @@
         <v>29</v>
       </c>
       <c r="N7">
-        <v>53.71147335634279</v>
+        <v>54.02451352198364</v>
       </c>
       <c r="O7" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 10:51:57
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>날짜</t>
   </si>
@@ -64,12 +64,12 @@
     <t>2025-12-05</t>
   </si>
   <si>
+    <t>058470.KS,0P0000ASU1,98886</t>
+  </si>
+  <si>
     <t>SamsungElec</t>
   </si>
   <si>
-    <t>058470.KS,0P0000ASU1,98886</t>
-  </si>
-  <si>
     <t>403870.KS,0P0001PE9K,566428</t>
   </si>
   <si>
@@ -82,12 +82,12 @@
     <t>240810.KS,0P00017YB3,330568</t>
   </si>
   <si>
+    <t>058470.KS</t>
+  </si>
+  <si>
     <t>005930.KS</t>
   </si>
   <si>
-    <t>058470.KS</t>
-  </si>
-  <si>
     <t>403870.KS</t>
   </si>
   <si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Pattern</t>
+  </si>
+  <si>
+    <t>📈 매수 관찰 구간입니다.</t>
   </si>
   <si>
     <t>⛔ 관망하십시오.</t>
@@ -528,28 +531,28 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>105100</v>
+        <v>65100</v>
       </c>
       <c r="E2">
-        <v>61.7</v>
+        <v>64.7</v>
       </c>
       <c r="F2">
-        <v>1.55</v>
+        <v>0.46</v>
       </c>
       <c r="G2">
         <v>60</v>
       </c>
       <c r="H2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="I2">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="J2">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="K2">
-        <v>56.6</v>
+        <v>63.7</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -558,10 +561,10 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>54.02451352198364</v>
+        <v>54.85170003294819</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -575,40 +578,40 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>66000</v>
+        <v>107400</v>
       </c>
       <c r="E3">
-        <v>67.09999999999999</v>
+        <v>60.4</v>
       </c>
       <c r="F3">
-        <v>2.33</v>
+        <v>6.87</v>
       </c>
       <c r="G3">
         <v>60</v>
       </c>
       <c r="H3">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I3">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J3">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="K3">
-        <v>56.6</v>
+        <v>58.5</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N3">
-        <v>54.02451352198364</v>
+        <v>54.85170003294819</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -622,40 +625,40 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>31000</v>
+        <v>30550</v>
       </c>
       <c r="E4">
-        <v>41.2</v>
+        <v>47.2</v>
       </c>
       <c r="F4">
-        <v>7.64</v>
+        <v>6.08</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H4">
         <v>50</v>
       </c>
       <c r="I4">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="J4">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="K4">
-        <v>52.4</v>
+        <v>51.7</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N4">
-        <v>54.02451352198364</v>
+        <v>54.85170003294819</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -669,40 +672,40 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>542000</v>
+        <v>537000</v>
       </c>
       <c r="E5">
-        <v>46.2</v>
+        <v>32.3</v>
       </c>
       <c r="F5">
-        <v>-0.37</v>
+        <v>1.32</v>
       </c>
       <c r="G5">
         <v>20</v>
       </c>
       <c r="H5">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="I5">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J5">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K5">
-        <v>47.4</v>
+        <v>48.9</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N5">
-        <v>54.02451352198364</v>
+        <v>54.85170003294819</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -716,40 +719,40 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>64400</v>
+        <v>65000</v>
       </c>
       <c r="E6">
-        <v>41.9</v>
+        <v>34.7</v>
       </c>
       <c r="F6">
-        <v>1.26</v>
+        <v>2.2</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
         <v>46</v>
       </c>
-      <c r="I6">
-        <v>50</v>
-      </c>
       <c r="J6">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="K6">
-        <v>45.2</v>
+        <v>40.9</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N6">
-        <v>54.02451352198364</v>
+        <v>54.85170003294819</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -763,40 +766,40 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>61900</v>
+        <v>61000</v>
       </c>
       <c r="E7">
-        <v>32.5</v>
+        <v>36.7</v>
       </c>
       <c r="F7">
-        <v>0.98</v>
+        <v>1.16</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I7">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="J7">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K7">
-        <v>44.6</v>
+        <v>40.9</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
       </c>
       <c r="M7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N7">
-        <v>54.02451352198364</v>
+        <v>54.85170003294819</v>
       </c>
       <c r="O7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 12:01:04
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -76,12 +76,12 @@
     <t>SK hynix</t>
   </si>
   <si>
+    <t>240810.KS,0P00017YB3,330568</t>
+  </si>
+  <si>
     <t>DB HiTek</t>
   </si>
   <si>
-    <t>240810.KS,0P00017YB3,330568</t>
-  </si>
-  <si>
     <t>058470.KS</t>
   </si>
   <si>
@@ -94,10 +94,10 @@
     <t>000660.KS</t>
   </si>
   <si>
+    <t>240810.KS</t>
+  </si>
+  <si>
     <t>000990.KS</t>
-  </si>
-  <si>
-    <t>240810.KS</t>
   </si>
   <si>
     <t>Pattern</t>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>54.85170003294819</v>
+        <v>54.86376272656823</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,13 +578,13 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>107400</v>
+        <v>107100</v>
       </c>
       <c r="E3">
-        <v>60.4</v>
+        <v>60.1</v>
       </c>
       <c r="F3">
-        <v>6.87</v>
+        <v>6.57</v>
       </c>
       <c r="G3">
         <v>60</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>54.85170003294819</v>
+        <v>54.86376272656823</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>54.85170003294819</v>
+        <v>54.86376272656823</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,13 +672,13 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>537000</v>
+        <v>535000</v>
       </c>
       <c r="E5">
-        <v>32.3</v>
+        <v>31.9</v>
       </c>
       <c r="F5">
-        <v>1.32</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>54.85170003294819</v>
+        <v>54.86376272656823</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -719,25 +719,25 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>65000</v>
+        <v>61000</v>
       </c>
       <c r="E6">
-        <v>34.7</v>
+        <v>36.7</v>
       </c>
       <c r="F6">
-        <v>2.2</v>
+        <v>1.16</v>
       </c>
       <c r="G6">
         <v>20</v>
       </c>
       <c r="H6">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="I6">
         <v>46</v>
       </c>
       <c r="J6">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="K6">
         <v>40.9</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>54.85170003294819</v>
+        <v>54.86376272656823</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -766,28 +766,28 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>61000</v>
+        <v>64100</v>
       </c>
       <c r="E7">
-        <v>36.7</v>
+        <v>31.8</v>
       </c>
       <c r="F7">
-        <v>1.16</v>
+        <v>0.79</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7">
+        <v>46</v>
+      </c>
+      <c r="I7">
+        <v>43</v>
+      </c>
+      <c r="J7">
         <v>60</v>
       </c>
-      <c r="I7">
-        <v>46</v>
-      </c>
-      <c r="J7">
-        <v>50</v>
-      </c>
       <c r="K7">
-        <v>40.9</v>
+        <v>39.7</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>54.85170003294819</v>
+        <v>54.86376272656823</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 12:21:03
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>54.86376272656823</v>
+        <v>54.84087454262382</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,13 +578,13 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>107100</v>
+        <v>107000</v>
       </c>
       <c r="E3">
-        <v>60.1</v>
+        <v>59.9</v>
       </c>
       <c r="F3">
-        <v>6.57</v>
+        <v>6.47</v>
       </c>
       <c r="G3">
         <v>60</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>54.86376272656823</v>
+        <v>54.84087454262382</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>54.86376272656823</v>
+        <v>54.84087454262382</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,13 +672,13 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>535000</v>
+        <v>538000</v>
       </c>
       <c r="E5">
-        <v>31.9</v>
+        <v>32.4</v>
       </c>
       <c r="F5">
-        <v>0.9399999999999999</v>
+        <v>1.51</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>54.86376272656823</v>
+        <v>54.84087454262382</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>54.86376272656823</v>
+        <v>54.84087454262382</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -766,13 +766,13 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>64100</v>
+        <v>64300</v>
       </c>
       <c r="E7">
-        <v>31.8</v>
+        <v>32.2</v>
       </c>
       <c r="F7">
-        <v>0.79</v>
+        <v>1.1</v>
       </c>
       <c r="G7">
         <v>20</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>54.86376272656823</v>
+        <v>54.84087454262382</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 13:00:26
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>63.7</v>
+        <v>63.6</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>54.84087454262382</v>
+        <v>54.82400714602223</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,13 +578,13 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>107000</v>
+        <v>107200</v>
       </c>
       <c r="E3">
-        <v>59.9</v>
+        <v>60.2</v>
       </c>
       <c r="F3">
-        <v>6.47</v>
+        <v>6.67</v>
       </c>
       <c r="G3">
         <v>60</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>58.5</v>
+        <v>58.4</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>54.84087454262382</v>
+        <v>54.82400714602223</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>51.7</v>
+        <v>51.6</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>54.84087454262382</v>
+        <v>54.82400714602223</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,13 +672,13 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>538000</v>
+        <v>536000</v>
       </c>
       <c r="E5">
-        <v>32.4</v>
+        <v>32.1</v>
       </c>
       <c r="F5">
-        <v>1.51</v>
+        <v>1.13</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>48.9</v>
+        <v>48.8</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>54.84087454262382</v>
+        <v>54.82400714602223</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>50</v>
       </c>
       <c r="K6">
-        <v>40.9</v>
+        <v>40.8</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>54.84087454262382</v>
+        <v>54.82400714602223</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -787,7 +787,7 @@
         <v>60</v>
       </c>
       <c r="K7">
-        <v>39.7</v>
+        <v>39.6</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>54.84087454262382</v>
+        <v>54.82400714602223</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 13:19:50
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>63.6</v>
+        <v>63.7</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>54.82400714602223</v>
+        <v>54.83846622768671</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,13 +578,13 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>107200</v>
+        <v>107300</v>
       </c>
       <c r="E3">
-        <v>60.2</v>
+        <v>60.3</v>
       </c>
       <c r="F3">
-        <v>6.67</v>
+        <v>6.77</v>
       </c>
       <c r="G3">
         <v>60</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>58.4</v>
+        <v>58.5</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>54.82400714602223</v>
+        <v>54.83846622768671</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>51.6</v>
+        <v>51.7</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>54.82400714602223</v>
+        <v>54.83846622768671</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,13 +672,13 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>536000</v>
+        <v>537000</v>
       </c>
       <c r="E5">
-        <v>32.1</v>
+        <v>32.3</v>
       </c>
       <c r="F5">
-        <v>1.13</v>
+        <v>1.32</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>48.8</v>
+        <v>48.9</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>54.82400714602223</v>
+        <v>54.83846622768671</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>50</v>
       </c>
       <c r="K6">
-        <v>40.8</v>
+        <v>40.9</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>54.82400714602223</v>
+        <v>54.83846622768671</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -766,13 +766,13 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>64300</v>
+        <v>64100</v>
       </c>
       <c r="E7">
-        <v>32.2</v>
+        <v>31.8</v>
       </c>
       <c r="F7">
-        <v>1.1</v>
+        <v>0.79</v>
       </c>
       <c r="G7">
         <v>20</v>
@@ -787,7 +787,7 @@
         <v>60</v>
       </c>
       <c r="K7">
-        <v>39.6</v>
+        <v>39.7</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>54.82400714602223</v>
+        <v>54.83846622768671</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 17:31:00
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -76,12 +76,12 @@
     <t>SK hynix</t>
   </si>
   <si>
+    <t>DB HiTek</t>
+  </si>
+  <si>
     <t>240810.KS,0P00017YB3,330568</t>
   </si>
   <si>
-    <t>DB HiTek</t>
-  </si>
-  <si>
     <t>058470.KS</t>
   </si>
   <si>
@@ -94,10 +94,10 @@
     <t>000660.KS</t>
   </si>
   <si>
+    <t>000990.KS</t>
+  </si>
+  <si>
     <t>240810.KS</t>
-  </si>
-  <si>
-    <t>000990.KS</t>
   </si>
   <si>
     <t>Pattern</t>
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>63.7</v>
+        <v>63.6</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>54.83846622768671</v>
+        <v>54.77309453746771</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -578,16 +578,16 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>107300</v>
+        <v>108400</v>
       </c>
       <c r="E3">
-        <v>60.3</v>
+        <v>61.6</v>
       </c>
       <c r="F3">
-        <v>6.77</v>
+        <v>7.86</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <v>53</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>58.5</v>
+        <v>55.4</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>54.83846622768671</v>
+        <v>54.77309453746771</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>51.7</v>
+        <v>51.6</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>54.83846622768671</v>
+        <v>54.77309453746771</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -672,13 +672,13 @@
         <v>25</v>
       </c>
       <c r="D5">
-        <v>537000</v>
+        <v>544000</v>
       </c>
       <c r="E5">
-        <v>32.3</v>
+        <v>33.8</v>
       </c>
       <c r="F5">
-        <v>1.32</v>
+        <v>2.64</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>48.9</v>
+        <v>48.8</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>54.83846622768671</v>
+        <v>54.77309453746771</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -719,28 +719,28 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>61000</v>
+        <v>64800</v>
       </c>
       <c r="E6">
-        <v>36.7</v>
+        <v>33.9</v>
       </c>
       <c r="F6">
-        <v>1.16</v>
+        <v>1.89</v>
       </c>
       <c r="G6">
         <v>20</v>
       </c>
       <c r="H6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I6">
         <v>46</v>
       </c>
       <c r="J6">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="K6">
-        <v>40.9</v>
+        <v>40.8</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>54.83846622768671</v>
+        <v>54.77309453746771</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -766,28 +766,28 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>64100</v>
+        <v>61000</v>
       </c>
       <c r="E7">
-        <v>31.8</v>
+        <v>36.7</v>
       </c>
       <c r="F7">
-        <v>0.79</v>
+        <v>1.16</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7">
+        <v>60</v>
+      </c>
+      <c r="I7">
         <v>46</v>
       </c>
-      <c r="I7">
-        <v>43</v>
-      </c>
       <c r="J7">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="K7">
-        <v>39.7</v>
+        <v>40.8</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>54.83846622768671</v>
+        <v>54.77309453746771</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 18:24:43
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>63.6</v>
+        <v>62.7</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>54.77309453746771</v>
+        <v>51.53902399942638</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>55.4</v>
+        <v>54.5</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>54.77309453746771</v>
+        <v>51.53902399942638</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>51.6</v>
+        <v>50.7</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>54.77309453746771</v>
+        <v>51.53902399942638</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>48.8</v>
+        <v>47.9</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>54.77309453746771</v>
+        <v>51.53902399942638</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>40.8</v>
+        <v>39.9</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>54.77309453746771</v>
+        <v>51.53902399942638</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -787,7 +787,7 @@
         <v>50</v>
       </c>
       <c r="K7">
-        <v>40.8</v>
+        <v>39.9</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>54.77309453746771</v>
+        <v>51.53902399942638</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 19:04:26
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>62.7</v>
+        <v>62.5</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>51.53902399942638</v>
+        <v>51.15965480231979</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>54.5</v>
+        <v>54.3</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>51.53902399942638</v>
+        <v>51.15965480231979</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>50.7</v>
+        <v>50.5</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>51.53902399942638</v>
+        <v>51.15965480231979</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>47.9</v>
+        <v>47.7</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>51.53902399942638</v>
+        <v>51.15965480231979</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>39.9</v>
+        <v>39.7</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>51.53902399942638</v>
+        <v>51.15965480231979</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -787,7 +787,7 @@
         <v>50</v>
       </c>
       <c r="K7">
-        <v>39.9</v>
+        <v>39.7</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>51.53902399942638</v>
+        <v>51.15965480231979</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-05 19:53:34
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>51.15965480231979</v>
+        <v>51.05762969290213</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>51.15965480231979</v>
+        <v>51.05762969290213</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>51.15965480231979</v>
+        <v>51.05762969290213</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>51.15965480231979</v>
+        <v>51.05762969290213</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>51.15965480231979</v>
+        <v>51.05762969290213</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>51.15965480231979</v>
+        <v>51.05762969290213</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-06 00:21:02
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -61,7 +61,7 @@
     <t>MACRO_SIGNAL</t>
   </si>
   <si>
-    <t>2025-12-05</t>
+    <t>2025-12-06</t>
   </si>
   <si>
     <t>058470.KS,0P0000ASU1,98886</t>
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>62.5</v>
+        <v>62.7</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>51.05762969290213</v>
+        <v>51.54219175917372</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>54.3</v>
+        <v>54.5</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>51.05762969290213</v>
+        <v>51.54219175917372</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>50.5</v>
+        <v>50.7</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>51.05762969290213</v>
+        <v>51.54219175917372</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>47.7</v>
+        <v>47.9</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>51.05762969290213</v>
+        <v>51.54219175917372</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>39.7</v>
+        <v>39.9</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>51.05762969290213</v>
+        <v>51.54219175917372</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -787,7 +787,7 @@
         <v>50</v>
       </c>
       <c r="K7">
-        <v>39.7</v>
+        <v>39.9</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>51.05762969290213</v>
+        <v>51.54219175917372</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-06 01:15:18
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>62.7</v>
+        <v>62.4</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>51.54219175917372</v>
+        <v>50.60178744571824</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>54.5</v>
+        <v>54.2</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>51.54219175917372</v>
+        <v>50.60178744571824</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>50.7</v>
+        <v>50.4</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>51.54219175917372</v>
+        <v>50.60178744571824</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>47.9</v>
+        <v>47.6</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>51.54219175917372</v>
+        <v>50.60178744571824</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>39.9</v>
+        <v>39.6</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>51.54219175917372</v>
+        <v>50.60178744571824</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -787,7 +787,7 @@
         <v>50</v>
       </c>
       <c r="K7">
-        <v>39.9</v>
+        <v>39.6</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>51.54219175917372</v>
+        <v>50.60178744571824</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-06 01:20:59
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>50.60178744571824</v>
+        <v>50.68470204858703</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>50.60178744571824</v>
+        <v>50.68470204858703</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>50.60178744571824</v>
+        <v>50.68470204858703</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>50.60178744571824</v>
+        <v>50.68470204858703</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>50.60178744571824</v>
+        <v>50.68470204858703</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>50.60178744571824</v>
+        <v>50.68470204858703</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-06 02:00:05
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -552,7 +552,7 @@
         <v>63</v>
       </c>
       <c r="K2">
-        <v>62.4</v>
+        <v>61.9</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,7 +561,7 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>50.68470204858703</v>
+        <v>49.16024380385575</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
@@ -599,7 +599,7 @@
         <v>76</v>
       </c>
       <c r="K3">
-        <v>54.2</v>
+        <v>53.7</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
@@ -608,7 +608,7 @@
         <v>30</v>
       </c>
       <c r="N3">
-        <v>50.68470204858703</v>
+        <v>49.16024380385575</v>
       </c>
       <c r="O3" t="s">
         <v>31</v>
@@ -646,7 +646,7 @@
         <v>50</v>
       </c>
       <c r="K4">
-        <v>50.4</v>
+        <v>49.9</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
@@ -655,7 +655,7 @@
         <v>30</v>
       </c>
       <c r="N4">
-        <v>50.68470204858703</v>
+        <v>49.16024380385575</v>
       </c>
       <c r="O4" t="s">
         <v>31</v>
@@ -693,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>47.6</v>
+        <v>47.1</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
@@ -702,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="N5">
-        <v>50.68470204858703</v>
+        <v>49.16024380385575</v>
       </c>
       <c r="O5" t="s">
         <v>31</v>
@@ -740,7 +740,7 @@
         <v>63</v>
       </c>
       <c r="K6">
-        <v>39.6</v>
+        <v>39.1</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
@@ -749,7 +749,7 @@
         <v>30</v>
       </c>
       <c r="N6">
-        <v>50.68470204858703</v>
+        <v>49.16024380385575</v>
       </c>
       <c r="O6" t="s">
         <v>31</v>
@@ -787,7 +787,7 @@
         <v>50</v>
       </c>
       <c r="K7">
-        <v>39.6</v>
+        <v>39.1</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -796,7 +796,7 @@
         <v>30</v>
       </c>
       <c r="N7">
-        <v>50.68470204858703</v>
+        <v>49.16024380385575</v>
       </c>
       <c r="O7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-06 21:20:02
</commit_message>
<xml_diff>
--- a/DECISION/국장_반도체_분석.xlsx
+++ b/DECISION/국장_반도체_분석.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>날짜</t>
   </si>
@@ -64,46 +64,43 @@
     <t>2025-12-06</t>
   </si>
   <si>
+    <t>SamsungElec</t>
+  </si>
+  <si>
     <t>058470.KS,0P0000ASU1,98886</t>
   </si>
   <si>
-    <t>SamsungElec</t>
-  </si>
-  <si>
     <t>403870.KS,0P0001PE9K,566428</t>
   </si>
   <si>
     <t>SK hynix</t>
   </si>
   <si>
+    <t>240810.KS,0P00017YB3,330568</t>
+  </si>
+  <si>
     <t>DB HiTek</t>
   </si>
   <si>
-    <t>240810.KS,0P00017YB3,330568</t>
+    <t>005930.KS</t>
   </si>
   <si>
     <t>058470.KS</t>
   </si>
   <si>
-    <t>005930.KS</t>
-  </si>
-  <si>
     <t>403870.KS</t>
   </si>
   <si>
     <t>000660.KS</t>
   </si>
   <si>
+    <t>240810.KS</t>
+  </si>
+  <si>
     <t>000990.KS</t>
   </si>
   <si>
-    <t>240810.KS</t>
-  </si>
-  <si>
     <t>Pattern</t>
-  </si>
-  <si>
-    <t>📈 매수 관찰 구간입니다.</t>
   </si>
   <si>
     <t>⛔ 관망하십시오.</t>
@@ -531,28 +528,28 @@
         <v>22</v>
       </c>
       <c r="D2">
-        <v>65100</v>
+        <v>108400</v>
       </c>
       <c r="E2">
-        <v>64.7</v>
+        <v>61.6</v>
       </c>
       <c r="F2">
-        <v>0.46</v>
+        <v>7.86</v>
       </c>
       <c r="G2">
+        <v>50</v>
+      </c>
+      <c r="H2">
+        <v>53</v>
+      </c>
+      <c r="I2">
         <v>60</v>
       </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2">
-        <v>73</v>
-      </c>
       <c r="J2">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="K2">
-        <v>61.9</v>
+        <v>54.7</v>
       </c>
       <c r="L2" t="s">
         <v>28</v>
@@ -561,10 +558,10 @@
         <v>29</v>
       </c>
       <c r="N2">
-        <v>49.16024380385575</v>
+        <v>52.28493729186943</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -578,40 +575,40 @@
         <v>23</v>
       </c>
       <c r="D3">
-        <v>108400</v>
+        <v>65400</v>
       </c>
       <c r="E3">
-        <v>61.6</v>
+        <v>61.7</v>
       </c>
       <c r="F3">
-        <v>7.86</v>
+        <v>-4.25</v>
       </c>
       <c r="G3">
         <v>50</v>
       </c>
       <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
         <v>53</v>
       </c>
-      <c r="I3">
-        <v>60</v>
-      </c>
       <c r="J3">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K3">
-        <v>53.7</v>
+        <v>51.9</v>
       </c>
       <c r="L3" t="s">
         <v>28</v>
       </c>
       <c r="M3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3">
+        <v>52.28493729186943</v>
+      </c>
+      <c r="O3" t="s">
         <v>30</v>
-      </c>
-      <c r="N3">
-        <v>49.16024380385575</v>
-      </c>
-      <c r="O3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -625,40 +622,40 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>30550</v>
+        <v>30300</v>
       </c>
       <c r="E4">
-        <v>47.2</v>
+        <v>43.3</v>
       </c>
       <c r="F4">
-        <v>6.08</v>
+        <v>0.17</v>
       </c>
       <c r="G4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>53</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
         <v>60</v>
       </c>
-      <c r="H4">
-        <v>50</v>
-      </c>
-      <c r="I4">
-        <v>43</v>
-      </c>
-      <c r="J4">
-        <v>50</v>
-      </c>
       <c r="K4">
-        <v>49.9</v>
+        <v>50.7</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
       </c>
       <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4">
+        <v>52.28493729186943</v>
+      </c>
+      <c r="O4" t="s">
         <v>30</v>
-      </c>
-      <c r="N4">
-        <v>49.16024380385575</v>
-      </c>
-      <c r="O4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -693,19 +690,19 @@
         <v>66</v>
       </c>
       <c r="K5">
-        <v>47.1</v>
+        <v>48.1</v>
       </c>
       <c r="L5" t="s">
         <v>28</v>
       </c>
       <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5">
+        <v>52.28493729186943</v>
+      </c>
+      <c r="O5" t="s">
         <v>30</v>
-      </c>
-      <c r="N5">
-        <v>49.16024380385575</v>
-      </c>
-      <c r="O5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -719,40 +716,40 @@
         <v>26</v>
       </c>
       <c r="D6">
-        <v>64800</v>
+        <v>61800</v>
       </c>
       <c r="E6">
-        <v>33.9</v>
+        <v>38</v>
       </c>
       <c r="F6">
-        <v>1.89</v>
+        <v>0.82</v>
       </c>
       <c r="G6">
         <v>20</v>
       </c>
       <c r="H6">
+        <v>53</v>
+      </c>
+      <c r="I6">
+        <v>53</v>
+      </c>
+      <c r="J6">
         <v>50</v>
       </c>
-      <c r="I6">
-        <v>46</v>
-      </c>
-      <c r="J6">
-        <v>63</v>
-      </c>
       <c r="K6">
-        <v>39.1</v>
+        <v>42.9</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
       </c>
       <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6">
+        <v>52.28493729186943</v>
+      </c>
+      <c r="O6" t="s">
         <v>30</v>
-      </c>
-      <c r="N6">
-        <v>49.16024380385575</v>
-      </c>
-      <c r="O6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -766,40 +763,40 @@
         <v>27</v>
       </c>
       <c r="D7">
-        <v>61000</v>
+        <v>64800</v>
       </c>
       <c r="E7">
-        <v>36.7</v>
+        <v>33.9</v>
       </c>
       <c r="F7">
-        <v>1.16</v>
+        <v>1.89</v>
       </c>
       <c r="G7">
         <v>20</v>
       </c>
       <c r="H7">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I7">
         <v>46</v>
       </c>
       <c r="J7">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="K7">
-        <v>39.1</v>
+        <v>40.1</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
       </c>
       <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7">
+        <v>52.28493729186943</v>
+      </c>
+      <c r="O7" t="s">
         <v>30</v>
-      </c>
-      <c r="N7">
-        <v>49.16024380385575</v>
-      </c>
-      <c r="O7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>